<commit_message>
Bug & dans les métadonnées
</commit_message>
<xml_diff>
--- a/critique2000.xlsx
+++ b/critique2000.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1820" yWindow="460" windowWidth="26960" windowHeight="16700" tabRatio="989"/>
+    <workbookView xWindow="820" yWindow="460" windowWidth="26960" windowHeight="16700" tabRatio="989"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil2" sheetId="3" r:id="rId1"/>
@@ -27240,8 +27240,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2069667072"/>
-        <c:axId val="-2051090064"/>
+        <c:axId val="-2050310352"/>
+        <c:axId val="-2052693840"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -28508,11 +28508,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2037232592"/>
-        <c:axId val="-2048710048"/>
+        <c:axId val="-2050637392"/>
+        <c:axId val="-2082345216"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2069667072"/>
+        <c:axId val="-2050310352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -28549,7 +28549,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -28568,7 +28568,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2051090064"/>
+        <c:crossAx val="-2052693840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -28578,7 +28578,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2051090064"/>
+        <c:axId val="-2052693840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -28628,12 +28628,12 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2069667072"/>
+        <c:crossAx val="-2050310352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2048710048"/>
+        <c:axId val="-2082345216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -28670,21 +28670,23 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2037232592"/>
+        <c:crossAx val="-2050637392"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="-2037232592"/>
+        <c:axId val="-2050637392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2048710048"/>
+        <c:crossAx val="-2082345216"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -32669,9 +32671,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H1841"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0"/>
+    <sheetView topLeftCell="A211" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="4" max="4" width="17.6640625" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" t="s">

</xml_diff>